<commit_message>
calorimetry : scripts : optimizer roughly done
</commit_message>
<xml_diff>
--- a/input/calorimetry/ds.1.dsc/data.xlsx
+++ b/input/calorimetry/ds.1.dsc/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" state="visible" r:id="rId2"/>
@@ -236,7 +236,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -252,7 +252,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -745,7 +745,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
calorimetry : scripts : postproc
</commit_message>
<xml_diff>
--- a/input/calorimetry/ds.1.dsc/data.xlsx
+++ b/input/calorimetry/ds.1.dsc/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" state="visible" r:id="rId2"/>
@@ -236,7 +236,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -466,10 +466,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -477,256 +477,285 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="N1" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="O1" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="P1" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>15.024977</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>0.069951</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>-0.001953538</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <v>15.049954</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>15.074931</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>15.099908</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>15.124885</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>15.149862</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>15.174839</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>15.199816</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>15.224793</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>15.24977</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>15.274747</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>15.299724</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>15.324701</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>15.349678</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <v>15.374655</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>0.069951</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.069513</v>
       </c>
       <c r="D3" s="0" t="n">
+        <v>0.002471029</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>15.074931</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>0.069854</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0.071474</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0.067108</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0.066289</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0.056026</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0.044493</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0.027882</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>0.009239</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>0.003057</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>0.002486</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>0.000906</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>4E-005</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>-0.001894</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>-0.001953538</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0.002471029</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>-0.00017689</v>
       </c>
       <c r="E4" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>15.099908</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.071474</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>0.000556654</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="E5" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>15.124885</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.067108</v>
+      </c>
+      <c r="D6" s="0" t="n">
         <v>0.00070773</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="E6" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>15.149862</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.066289</v>
+      </c>
+      <c r="D7" s="0" t="n">
         <v>0.001854236</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="E7" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>15.174839</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.056026</v>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>0.001081072</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="E8" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>15.199816</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.044493</v>
+      </c>
+      <c r="D9" s="0" t="n">
         <v>0.000473122</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="E9" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>15.224793</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.027882</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>0.00106313</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="E10" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>15.24977</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.009239</v>
+      </c>
+      <c r="D11" s="0" t="n">
         <v>0.000271799</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="E11" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>15.274747</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.003057</v>
+      </c>
+      <c r="D12" s="0" t="n">
         <v>0.001168423</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="E12" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>15.299724</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.002486</v>
+      </c>
+      <c r="D13" s="0" t="n">
         <v>0.000232129</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="E13" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>15.324701</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.000906</v>
+      </c>
+      <c r="D14" s="0" t="n">
         <v>0.000917353</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="E14" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>15.349678</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>4E-005</v>
+      </c>
+      <c r="D15" s="0" t="n">
         <v>0.001269958</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="E15" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>15.374655</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>-0.001894</v>
+      </c>
+      <c r="D16" s="0" t="n">
         <v>-0.000397241</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="N5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-      <c r="P5" s="0" t="n">
-        <v>1E-006</v>
-      </c>
-    </row>
+      <c r="E16" s="0" t="n">
+        <v>1E-006</v>
+      </c>
+    </row>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>